<commit_message>
Update on 20241204 part 3
</commit_message>
<xml_diff>
--- a/各地组播源汇总/江苏.xlsx
+++ b/各地组播源汇总/江苏.xlsx
@@ -4,15 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="165" windowWidth="19395" windowHeight="7575" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="195" windowWidth="19395" windowHeight="7545" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="电信组播-非239.49.0网段(可能只能江苏内部可看)" sheetId="9" r:id="rId1"/>
-    <sheet name="电信组播-239.49.0网段(全网可看)" sheetId="8" r:id="rId2"/>
-    <sheet name="可用IP地址" sheetId="7" r:id="rId3"/>
+    <sheet name="电信组播-239.49.0网段(全网可看-标清)" sheetId="8" r:id="rId2"/>
+    <sheet name="电信组播-239.49.8网段(全网可看-高清)" sheetId="11" r:id="rId3"/>
+    <sheet name="可用IP地址" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'电信组播-239.49.0网段(全网可看)'!$A$1:$E$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'电信组播-239.49.0网段(全网可看-标清)'!$A$1:$E$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'电信组播-239.49.8网段(全网可看-高清)'!$A$1:$E$226</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'电信组播-非239.49.0网段(可能只能江苏内部可看)'!$A$1:$E$379</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2487" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3622" uniqueCount="746">
   <si>
     <t>/rtp/239.49.1.124:6000</t>
   </si>
@@ -2194,13 +2196,109 @@
   </si>
   <si>
     <t>/rtp/239.49.0.209:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.0.238:8000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新沂综合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/rtp/239.49.0.136:9976</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.107:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.108:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.118:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.120:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.117:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.122:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.30:8000</t>
+  </si>
+  <si>
+    <t>wx.puchengyu2009.top:9999</t>
+  </si>
+  <si>
+    <t>st.sportbabytoy.com:9999</t>
+  </si>
+  <si>
+    <t>dell.puchengyu2009.top:9999</t>
+  </si>
+  <si>
+    <t>,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>南京文旅纪录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盐城综合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>风云剧场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>风云音乐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>央视台球</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.85:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.93:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.94:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.89:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.92:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.91:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.87:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.32:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.88:8000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2213,6 +2311,22 @@
       <sz val="9"/>
       <name val="宋体"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -2239,18 +2353,171 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -18087,9 +18354,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -19868,9 +20135,9 @@
         <v>605</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="1" t="s">
-        <v>700</v>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A105" t="s">
+        <v>695</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>688</v>
@@ -19881,13 +20148,13 @@
       <c r="D105" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="E105" s="1" t="s">
-        <v>699</v>
+      <c r="E105" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>688</v>
@@ -19899,12 +20166,12 @@
         <v>690</v>
       </c>
       <c r="E106" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>688</v>
@@ -19916,12 +20183,12 @@
         <v>690</v>
       </c>
       <c r="E107" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>688</v>
@@ -19933,12 +20200,12 @@
         <v>690</v>
       </c>
       <c r="E108" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>688</v>
@@ -19950,12 +20217,12 @@
         <v>690</v>
       </c>
       <c r="E109" t="s">
-        <v>693</v>
+        <v>702</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>688</v>
@@ -19967,12 +20234,12 @@
         <v>690</v>
       </c>
       <c r="E110" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>688</v>
@@ -19984,12 +20251,12 @@
         <v>690</v>
       </c>
       <c r="E111" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>688</v>
@@ -20001,12 +20268,12 @@
         <v>690</v>
       </c>
       <c r="E112" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>688</v>
@@ -20018,12 +20285,12 @@
         <v>690</v>
       </c>
       <c r="E113" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>688</v>
@@ -20035,12 +20302,12 @@
         <v>690</v>
       </c>
       <c r="E114" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A115" t="s">
-        <v>711</v>
+      <c r="A115" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>688</v>
@@ -20051,13 +20318,13 @@
       <c r="D115" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="E115" t="s">
-        <v>712</v>
+      <c r="E115" s="1" t="s">
+        <v>719</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A116" t="s">
-        <v>713</v>
+      <c r="A116" s="1" t="s">
+        <v>718</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>688</v>
@@ -20068,35 +20335,3923 @@
       <c r="D116" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="E116" t="s">
-        <v>714</v>
+      <c r="E116" s="1" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
+        <v>713</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="E117" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A118" t="s">
         <v>715</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="E117" t="s">
+      <c r="B118" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="E118" t="s">
         <v>716</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E104"/>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="E116">
+    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E115">
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E226"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A32" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A34" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A36" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A38" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A43" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A46" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A52" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A54" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A55" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A56" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A57" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A58" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A59" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A60" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A61" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A62" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A63" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A64" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A65" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A66" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A67" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A68" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A69" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A70" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A71" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A72" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A73" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A74" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A75" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A76" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A77" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A78" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A79" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A80" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A81" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A82" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A83" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A84" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A85" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A86" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A87" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A88" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A89" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A90" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A91" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A92" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A93" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A94" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A95" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A96" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A97" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A98" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A99" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A100" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A101" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A102" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A103" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A104" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A105" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A106" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A107" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A108" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A109" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A110" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A111" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A112" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A113" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A114" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A115" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A116" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A117" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A118" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A119" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A120" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A121" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A122" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A123" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A124" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A125" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A126" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A127" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A128" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E128" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A129" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A130" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A131" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A132" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A133" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A134" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A135" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A136" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A137" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E137" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A138" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A139" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A140" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A141" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A142" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A143" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A144" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A145" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E145" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A146" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E146" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A147" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A148" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A149" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A150" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A151" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A152" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A153" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A154" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E154" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A155" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E155" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A156" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A157" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A158" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A159" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A160" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A161" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A162" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A163" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E163" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A164" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E164" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A165" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A166" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A167" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A168" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A169" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A170" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A171" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A172" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A173" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E173" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A174" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A175" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A176" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A177" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A178" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A179" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A180" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A181" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E181" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A182" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D182" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E182" s="5" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A183" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D183" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A184" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D184" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A185" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D185" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A186" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D186" s="4" t="s">
+        <v>727</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A187" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D187" s="4" t="s">
+        <v>728</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A188" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D188" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A189" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D189" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A190" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D190" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A191" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D191" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E191" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A192" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D192" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A193" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D193" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A194" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D194" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A195" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D195" s="4" t="s">
+        <v>727</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A196" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>728</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A197" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D197" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A198" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D198" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A199" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A200" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E200" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A201" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A202" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A203" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A204" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D204" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A205" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D205" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A206" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A207" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A208" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D208" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E208" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A209" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D209" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E209" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A210" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A211" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A212" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A213" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A214" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D214" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A215" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D215" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A216" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A217" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D217" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A218" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D218" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E218" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A219" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D219" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A220" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D220" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A221" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D221" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A222" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D222" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A223" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D223" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A224" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D224" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A225" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A226" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D226" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E226"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update on 20241205 part 4
</commit_message>
<xml_diff>
--- a/各地组播源汇总/江苏.xlsx
+++ b/各地组播源汇总/江苏.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="195" windowWidth="19395" windowHeight="7545" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="225" windowWidth="19395" windowHeight="7515" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="电信组播-非239.49.0网段(可能只能江苏内部可看)" sheetId="9" r:id="rId1"/>
@@ -14,7 +14,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'电信组播-239.49.0网段(全网可看-标清)'!$A$1:$E$104</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'电信组播-239.49.8网段(全网可看-高清)'!$A$1:$E$226</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'电信组播-239.49.8网段(全网可看-高清)'!$A$1:$E$145</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'电信组播-非239.49.0网段(可能只能江苏内部可看)'!$A$1:$E$379</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3622" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3217" uniqueCount="743">
   <si>
     <t>/rtp/239.49.1.124:6000</t>
   </si>
@@ -2134,14 +2134,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/rtp/239.49.8.116:8000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>苏州生活资讯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>泰州新闻综合</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2245,10 +2237,6 @@
   </si>
   <si>
     <t>http://</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>南京文旅纪录</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2298,7 +2286,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2311,22 +2299,6 @@
       <sz val="9"/>
       <name val="宋体"/>
       <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -2353,7 +2325,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2363,140 +2335,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -18356,7 +18199,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -20205,7 +20050,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>688</v>
@@ -20217,12 +20062,12 @@
         <v>690</v>
       </c>
       <c r="E109" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>688</v>
@@ -20234,12 +20079,12 @@
         <v>690</v>
       </c>
       <c r="E110" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>688</v>
@@ -20251,12 +20096,12 @@
         <v>690</v>
       </c>
       <c r="E111" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>688</v>
@@ -20268,12 +20113,12 @@
         <v>690</v>
       </c>
       <c r="E112" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>688</v>
@@ -20285,12 +20130,12 @@
         <v>690</v>
       </c>
       <c r="E113" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>688</v>
@@ -20302,7 +20147,7 @@
         <v>690</v>
       </c>
       <c r="E114" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.15">
@@ -20319,12 +20164,12 @@
         <v>690</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>688</v>
@@ -20336,12 +20181,12 @@
         <v>690</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>688</v>
@@ -20353,12 +20198,12 @@
         <v>690</v>
       </c>
       <c r="E117" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>688</v>
@@ -20370,17 +20215,17 @@
         <v>690</v>
       </c>
       <c r="E118" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E104"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E116">
-    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E115">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20388,7 +20233,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E226"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -20423,16 +20268,16 @@
         <v>165</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -20440,16 +20285,16 @@
         <v>165</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -20457,16 +20302,16 @@
         <v>165</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -20474,16 +20319,16 @@
         <v>165</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -20491,16 +20336,16 @@
         <v>165</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -20508,16 +20353,16 @@
         <v>165</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -20525,16 +20370,16 @@
         <v>165</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -20542,16 +20387,16 @@
         <v>165</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -20559,16 +20404,16 @@
         <v>165</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -20576,16 +20421,16 @@
         <v>166</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -20593,16 +20438,16 @@
         <v>166</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -20610,16 +20455,16 @@
         <v>166</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -20627,16 +20472,16 @@
         <v>166</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -20644,16 +20489,16 @@
         <v>166</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
@@ -20661,16 +20506,16 @@
         <v>166</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -20678,16 +20523,16 @@
         <v>166</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
@@ -20695,16 +20540,16 @@
         <v>166</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
@@ -20712,16 +20557,16 @@
         <v>166</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -20729,16 +20574,16 @@
         <v>168</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
@@ -20746,16 +20591,16 @@
         <v>168</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -20763,16 +20608,16 @@
         <v>168</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -20780,16 +20625,16 @@
         <v>168</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
@@ -20797,16 +20642,16 @@
         <v>168</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
@@ -20814,16 +20659,16 @@
         <v>168</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
@@ -20831,16 +20676,16 @@
         <v>168</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
@@ -20848,16 +20693,16 @@
         <v>168</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
@@ -20865,16 +20710,16 @@
         <v>168</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -20882,16 +20727,16 @@
         <v>381</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
@@ -20899,16 +20744,16 @@
         <v>381</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
@@ -20916,16 +20761,16 @@
         <v>381</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
@@ -20933,16 +20778,16 @@
         <v>381</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
@@ -20950,16 +20795,16 @@
         <v>381</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
@@ -20967,16 +20812,16 @@
         <v>381</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
@@ -20984,16 +20829,16 @@
         <v>381</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
@@ -21001,16 +20846,16 @@
         <v>381</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
@@ -21018,16 +20863,16 @@
         <v>381</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
@@ -21035,16 +20880,16 @@
         <v>167</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
@@ -21052,16 +20897,16 @@
         <v>167</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
@@ -21069,16 +20914,16 @@
         <v>167</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
@@ -21086,16 +20931,16 @@
         <v>167</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
@@ -21103,16 +20948,16 @@
         <v>167</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
@@ -21120,16 +20965,16 @@
         <v>167</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
@@ -21137,16 +20982,16 @@
         <v>167</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
@@ -21154,16 +20999,16 @@
         <v>167</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
@@ -21171,16 +21016,16 @@
         <v>167</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
@@ -21188,16 +21033,16 @@
         <v>173</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
@@ -21205,16 +21050,16 @@
         <v>173</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
@@ -21222,16 +21067,16 @@
         <v>173</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
@@ -21239,16 +21084,16 @@
         <v>173</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
@@ -21256,16 +21101,16 @@
         <v>173</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
@@ -21273,16 +21118,16 @@
         <v>173</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
@@ -21290,16 +21135,16 @@
         <v>173</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
@@ -21307,16 +21152,16 @@
         <v>173</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
@@ -21324,2927 +21169,1550 @@
         <v>173</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>363</v>
+        <v>730</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>53</v>
+        <v>724</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>363</v>
+        <v>730</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>53</v>
+        <v>724</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>363</v>
+        <v>730</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>53</v>
+        <v>724</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>363</v>
+        <v>730</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>53</v>
+        <v>724</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>363</v>
+        <v>730</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>53</v>
+        <v>724</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>363</v>
+        <v>730</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>53</v>
+        <v>724</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>363</v>
+        <v>730</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>53</v>
+        <v>724</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>363</v>
+        <v>730</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>53</v>
+        <v>724</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>363</v>
+        <v>730</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>53</v>
+        <v>724</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>732</v>
+        <v>205</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>51</v>
+      <c r="E65" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>732</v>
+        <v>205</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>51</v>
+        <v>734</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>732</v>
+        <v>205</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>51</v>
+        <v>734</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>732</v>
+        <v>205</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>51</v>
+        <v>734</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>732</v>
+        <v>205</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>51</v>
+        <v>734</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>732</v>
+        <v>205</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>51</v>
+        <v>734</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>732</v>
+        <v>205</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>51</v>
+        <v>734</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>732</v>
+        <v>205</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>51</v>
+        <v>734</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>732</v>
+        <v>205</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>51</v>
+        <v>734</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>732</v>
+        <v>213</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>55</v>
+      <c r="E74" t="s">
+        <v>735</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>732</v>
+        <v>213</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>55</v>
+        <v>735</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>732</v>
+        <v>213</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>55</v>
+        <v>735</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>732</v>
+        <v>213</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>55</v>
+        <v>735</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>732</v>
+        <v>213</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>55</v>
+        <v>735</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>732</v>
+        <v>213</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>55</v>
+        <v>735</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>732</v>
+        <v>213</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>55</v>
+        <v>735</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>732</v>
+        <v>213</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>55</v>
+        <v>735</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>732</v>
+        <v>213</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E82" s="1" t="s">
-        <v>55</v>
+      <c r="E82" t="s">
+        <v>735</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>365</v>
+        <v>278</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>42</v>
+      <c r="E83" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>365</v>
+        <v>278</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>42</v>
+        <v>736</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>365</v>
+        <v>278</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>42</v>
+        <v>736</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>365</v>
+        <v>278</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>42</v>
+        <v>736</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>365</v>
+        <v>278</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>42</v>
+        <v>736</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
-        <v>365</v>
+        <v>278</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>42</v>
+        <v>736</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>365</v>
+        <v>278</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>42</v>
+        <v>736</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>365</v>
+        <v>278</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>42</v>
+        <v>736</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
-        <v>365</v>
+        <v>278</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E91" s="1" t="s">
-        <v>42</v>
+      <c r="E91" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
-        <v>700</v>
+        <v>731</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E92" s="1" t="s">
-        <v>699</v>
+      <c r="E92" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>700</v>
+        <v>731</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>699</v>
+        <v>737</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
-        <v>700</v>
+        <v>731</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>699</v>
+        <v>737</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
-        <v>700</v>
+        <v>731</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>699</v>
+        <v>737</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
-        <v>700</v>
+        <v>731</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>699</v>
+        <v>737</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
-        <v>700</v>
+        <v>731</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>699</v>
+        <v>737</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>700</v>
+        <v>731</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>699</v>
+        <v>737</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>700</v>
+        <v>731</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>699</v>
+        <v>737</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>700</v>
+        <v>731</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E100" s="1" t="s">
-        <v>699</v>
+      <c r="E100" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>700</v>
+        <v>732</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E101" s="1" t="s">
-        <v>62</v>
+      <c r="E101" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
-        <v>700</v>
+        <v>732</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>62</v>
+        <v>738</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
-        <v>700</v>
+        <v>732</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>62</v>
+        <v>738</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
-        <v>700</v>
+        <v>732</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>62</v>
+        <v>738</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
-        <v>700</v>
+        <v>732</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>62</v>
+        <v>738</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A106" s="1" t="s">
-        <v>700</v>
+        <v>732</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>62</v>
+        <v>738</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>700</v>
+        <v>732</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>62</v>
+        <v>738</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
-        <v>700</v>
+        <v>732</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>62</v>
+        <v>738</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>700</v>
+        <v>732</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>62</v>
+        <v>738</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>733</v>
+        <v>211</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>726</v>
+      <c r="E110" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
-        <v>733</v>
+        <v>211</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>726</v>
+        <v>739</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>733</v>
+        <v>211</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>726</v>
+        <v>739</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>733</v>
+        <v>211</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>726</v>
+        <v>739</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>733</v>
+        <v>211</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>726</v>
+        <v>739</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>733</v>
+        <v>211</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>726</v>
+        <v>739</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>733</v>
+        <v>211</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>726</v>
+        <v>739</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
-        <v>733</v>
+        <v>211</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>726</v>
+        <v>739</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
-        <v>733</v>
+        <v>211</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E118" s="1" t="s">
-        <v>726</v>
+      <c r="E118" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>350</v>
+        <v>207</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E119" s="1" t="s">
-        <v>36</v>
+      <c r="E119" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
-        <v>350</v>
+        <v>207</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>36</v>
+        <v>740</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
-        <v>350</v>
+        <v>207</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>36</v>
+        <v>740</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>350</v>
+        <v>207</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>36</v>
+        <v>740</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>350</v>
+        <v>207</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>36</v>
+        <v>740</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>350</v>
+        <v>207</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>36</v>
+        <v>740</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
-        <v>350</v>
+        <v>207</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>36</v>
+        <v>740</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>350</v>
+        <v>207</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>36</v>
+        <v>740</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>350</v>
+        <v>207</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E127" s="1" t="s">
-        <v>36</v>
+      <c r="E127" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
-        <v>205</v>
+        <v>733</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E128" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
-        <v>205</v>
+        <v>733</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>205</v>
+        <v>733</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
-        <v>205</v>
+        <v>733</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
-        <v>205</v>
+        <v>733</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>205</v>
+        <v>733</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
-        <v>205</v>
+        <v>733</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
-        <v>205</v>
+        <v>733</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>205</v>
+        <v>733</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E137" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A143" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A145" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E145" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A146" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E146" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A147" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A148" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D148" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A149" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D149" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A150" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A151" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D151" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A152" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D152" s="2" t="s">
-        <v>729</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A153" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D153" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A154" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D154" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E154" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A155" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D155" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E155" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A156" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D156" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A157" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D157" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A158" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D158" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A159" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D159" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A160" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D160" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A161" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D161" s="2" t="s">
-        <v>729</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A162" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D162" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A163" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D163" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E163" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A164" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D164" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E164" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A165" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D165" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A166" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D166" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A167" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A168" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D168" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A169" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D169" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A170" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D170" s="2" t="s">
-        <v>729</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A171" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D171" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A172" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D172" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A173" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C173" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D173" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E173" t="s">
+      <c r="E145" s="1" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A174" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D174" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A175" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D175" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A176" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D176" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A177" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D177" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A178" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D178" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A179" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D179" s="2" t="s">
-        <v>729</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A180" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D180" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A181" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D181" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E181" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A182" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="B182" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C182" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D182" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E182" s="5" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A183" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="B183" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D183" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E183" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A184" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C184" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D184" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E184" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A185" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C185" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D185" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E185" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A186" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D186" s="4" t="s">
-        <v>727</v>
-      </c>
-      <c r="E186" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A187" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C187" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D187" s="4" t="s">
-        <v>728</v>
-      </c>
-      <c r="E187" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A188" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D188" s="4" t="s">
-        <v>729</v>
-      </c>
-      <c r="E188" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A189" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D189" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E189" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A190" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C190" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D190" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E190" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A191" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B191" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D191" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E191" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A192" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D192" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E192" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A193" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B193" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D193" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E193" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A194" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C194" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D194" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E194" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A195" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D195" s="4" t="s">
-        <v>727</v>
-      </c>
-      <c r="E195" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A196" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B196" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C196" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D196" s="4" t="s">
-        <v>728</v>
-      </c>
-      <c r="E196" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A197" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B197" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D197" s="4" t="s">
-        <v>729</v>
-      </c>
-      <c r="E197" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A198" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B198" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D198" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E198" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A199" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B199" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C199" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="D199" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E199" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A200" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C200" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D200" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E200" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A201" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C201" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D201" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E201" s="1" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A202" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C202" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D202" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E202" s="1" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A203" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C203" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D203" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E203" s="1" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A204" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C204" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D204" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A205" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D205" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="E205" s="1" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A206" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C206" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D206" s="2" t="s">
-        <v>729</v>
-      </c>
-      <c r="E206" s="1" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A207" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C207" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D207" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E207" s="1" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A208" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C208" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D208" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E208" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A209" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C209" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D209" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E209" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A210" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C210" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D210" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E210" s="1" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A211" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C211" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D211" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A212" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C212" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D212" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A213" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C213" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D213" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A214" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C214" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D214" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="E214" s="1" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A215" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C215" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D215" s="2" t="s">
-        <v>729</v>
-      </c>
-      <c r="E215" s="1" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A216" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D216" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A217" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C217" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D217" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E217" s="1" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A218" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C218" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D218" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E218" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A219" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C219" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D219" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A220" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C220" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D220" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A221" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D221" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A222" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D222" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="E222" s="1" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A223" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C223" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D223" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A224" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C224" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D224" s="2" t="s">
-        <v>729</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A225" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C225" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D225" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E225" s="1" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A226" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C226" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D226" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>745</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E226"/>
+  <autoFilter ref="A1:E145"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update on 20241205 part 5
</commit_message>
<xml_diff>
--- a/各地组播源汇总/江苏.xlsx
+++ b/各地组播源汇总/江苏.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'电信组播-239.49.0网段(全网可看-标清)'!$A$1:$E$104</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'电信组播-239.49.8网段(全网可看-高清)'!$A$1:$E$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'电信组播-239.49.8网段(全网可看-高清)'!$A$1:$E$172</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'电信组播-非239.49.0网段(可能只能江苏内部可看)'!$A$1:$E$379</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3217" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3352" uniqueCount="746">
   <si>
     <t>/rtp/239.49.1.124:6000</t>
   </si>
@@ -2280,6 +2280,15 @@
   </si>
   <si>
     <t>/rtp/239.49.8.88:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.84:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.86:8000</t>
+  </si>
+  <si>
+    <t>/rtp/239.49.8.90:8000</t>
   </si>
 </sst>
 </file>
@@ -20233,9 +20242,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E145"/>
+  <dimension ref="A1:E172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -21334,162 +21345,162 @@
         <v>724</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E65" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E65" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>725</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>726</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>727</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>734</v>
+        <v>743</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>728</v>
@@ -21501,12 +21512,12 @@
         <v>21</v>
       </c>
       <c r="E74" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>728</v>
@@ -21518,12 +21529,12 @@
         <v>22</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>728</v>
@@ -21535,12 +21546,12 @@
         <v>23</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>728</v>
@@ -21552,12 +21563,12 @@
         <v>24</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>728</v>
@@ -21569,12 +21580,12 @@
         <v>725</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>728</v>
@@ -21586,12 +21597,12 @@
         <v>726</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>728</v>
@@ -21603,12 +21614,12 @@
         <v>727</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>728</v>
@@ -21620,12 +21631,12 @@
         <v>105</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>728</v>
@@ -21636,13 +21647,13 @@
       <c r="D82" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E82" t="s">
-        <v>735</v>
+      <c r="E82" s="1" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>278</v>
+        <v>213</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>728</v>
@@ -21654,12 +21665,12 @@
         <v>21</v>
       </c>
       <c r="E83" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>278</v>
+        <v>213</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>728</v>
@@ -21671,12 +21682,12 @@
         <v>22</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>278</v>
+        <v>213</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>728</v>
@@ -21688,12 +21699,12 @@
         <v>23</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>278</v>
+        <v>213</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>728</v>
@@ -21705,12 +21716,12 @@
         <v>24</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>278</v>
+        <v>213</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>728</v>
@@ -21722,12 +21733,12 @@
         <v>725</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
-        <v>278</v>
+        <v>213</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>728</v>
@@ -21739,12 +21750,12 @@
         <v>726</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>278</v>
+        <v>213</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>728</v>
@@ -21756,12 +21767,12 @@
         <v>727</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>278</v>
+        <v>213</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>728</v>
@@ -21773,12 +21784,12 @@
         <v>105</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
-        <v>278</v>
+        <v>213</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>728</v>
@@ -21790,12 +21801,12 @@
         <v>106</v>
       </c>
       <c r="E91" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
-        <v>731</v>
+        <v>278</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>728</v>
@@ -21807,12 +21818,12 @@
         <v>21</v>
       </c>
       <c r="E92" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>731</v>
+        <v>278</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>728</v>
@@ -21824,12 +21835,12 @@
         <v>22</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
-        <v>731</v>
+        <v>278</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>728</v>
@@ -21841,12 +21852,12 @@
         <v>23</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
-        <v>731</v>
+        <v>278</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>728</v>
@@ -21858,12 +21869,12 @@
         <v>24</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
-        <v>731</v>
+        <v>278</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>728</v>
@@ -21875,12 +21886,12 @@
         <v>725</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
-        <v>731</v>
+        <v>278</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>728</v>
@@ -21892,12 +21903,12 @@
         <v>726</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>731</v>
+        <v>278</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>728</v>
@@ -21909,12 +21920,12 @@
         <v>727</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>731</v>
+        <v>278</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>728</v>
@@ -21926,12 +21937,12 @@
         <v>105</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>731</v>
+        <v>278</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>728</v>
@@ -21943,12 +21954,12 @@
         <v>106</v>
       </c>
       <c r="E100" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>728</v>
@@ -21960,12 +21971,12 @@
         <v>21</v>
       </c>
       <c r="E101" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>728</v>
@@ -21977,12 +21988,12 @@
         <v>22</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>728</v>
@@ -21994,12 +22005,12 @@
         <v>23</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>728</v>
@@ -22011,12 +22022,12 @@
         <v>24</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>728</v>
@@ -22028,12 +22039,12 @@
         <v>725</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A106" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>728</v>
@@ -22045,12 +22056,12 @@
         <v>726</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>728</v>
@@ -22062,12 +22073,12 @@
         <v>727</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>728</v>
@@ -22079,12 +22090,12 @@
         <v>105</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>728</v>
@@ -22095,13 +22106,13 @@
       <c r="D109" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E109" s="1" t="s">
-        <v>738</v>
+      <c r="E109" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>211</v>
+        <v>732</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>728</v>
@@ -22113,12 +22124,12 @@
         <v>21</v>
       </c>
       <c r="E110" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
-        <v>211</v>
+        <v>732</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>728</v>
@@ -22130,12 +22141,12 @@
         <v>22</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>211</v>
+        <v>732</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>728</v>
@@ -22147,12 +22158,12 @@
         <v>23</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>211</v>
+        <v>732</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>728</v>
@@ -22164,12 +22175,12 @@
         <v>24</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>211</v>
+        <v>732</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>728</v>
@@ -22181,12 +22192,12 @@
         <v>725</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>211</v>
+        <v>732</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>728</v>
@@ -22198,12 +22209,12 @@
         <v>726</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>211</v>
+        <v>732</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>728</v>
@@ -22215,12 +22226,12 @@
         <v>727</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
-        <v>211</v>
+        <v>732</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>728</v>
@@ -22232,12 +22243,12 @@
         <v>105</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
-        <v>211</v>
+        <v>732</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>728</v>
@@ -22248,319 +22259,319 @@
       <c r="D118" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E118" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E118" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>207</v>
+        <v>395</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E119" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E119" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
-        <v>207</v>
+        <v>395</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.15">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
-        <v>207</v>
+        <v>395</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.15">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>207</v>
+        <v>395</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.15">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>207</v>
+        <v>395</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>725</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.15">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>207</v>
+        <v>395</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>726</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.15">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
-        <v>207</v>
+        <v>395</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>727</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.15">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>207</v>
+        <v>395</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.15">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>207</v>
+        <v>395</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E127" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E127" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
-        <v>733</v>
+        <v>210</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E128" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E128" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
-        <v>733</v>
+        <v>210</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.15">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>733</v>
+        <v>210</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.15">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
-        <v>733</v>
+        <v>210</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.15">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
-        <v>733</v>
+        <v>210</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>725</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.15">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>733</v>
+        <v>210</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>726</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.15">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
-        <v>733</v>
+        <v>210</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>727</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.15">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
-        <v>733</v>
+        <v>210</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.15">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>733</v>
+        <v>210</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>729</v>
+        <v>689</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>728</v>
@@ -22572,12 +22583,12 @@
         <v>21</v>
       </c>
       <c r="E137" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>728</v>
@@ -22589,12 +22600,12 @@
         <v>22</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>728</v>
@@ -22606,12 +22617,12 @@
         <v>23</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>728</v>
@@ -22623,12 +22634,12 @@
         <v>24</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>728</v>
@@ -22640,12 +22651,12 @@
         <v>725</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>728</v>
@@ -22657,12 +22668,12 @@
         <v>726</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A143" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>728</v>
@@ -22674,12 +22685,12 @@
         <v>727</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>728</v>
@@ -22691,12 +22702,12 @@
         <v>105</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A145" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>728</v>
@@ -22707,12 +22718,471 @@
       <c r="D145" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E145" s="1" t="s">
+      <c r="E145" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A146" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E146" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A147" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A148" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A149" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A150" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A151" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A152" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A153" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A154" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E154" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A155" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E155" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A156" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A157" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A158" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A159" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A160" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A161" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A162" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A163" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A164" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E164" t="s">
         <v>742</v>
       </c>
     </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A165" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A166" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A167" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A168" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A169" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A170" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A171" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A172" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E145"/>
+  <autoFilter ref="A1:E172"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>